<commit_message>
BTE Type attribute list: updated list of attributes relevant to process (now 99% complete)
</commit_message>
<xml_diff>
--- a/documentation/ProcessAttributeShortList.xlsx
+++ b/documentation/ProcessAttributeShortList.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://envester-my.sharepoint.com/personal/erlend_fjosna_envester_no/Documents/Envester/Material/BTE_MB/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="14_{0EC83A20-7867-4CA1-8EB2-19A4F162186E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="74" documentId="14_{0EC83A20-7867-4CA1-8EB2-19A4F162186E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{9F4BED6D-0204-4F83-97D8-E8AA3CF2957B}"/>
   <bookViews>
-    <workbookView xWindow="45435" yWindow="-45" windowWidth="26880" windowHeight="19815" xr2:uid="{27BA6BDA-B2D9-405F-9DD6-DE44F0E7623F}"/>
+    <workbookView xWindow="9300" yWindow="795" windowWidth="26880" windowHeight="19815" xr2:uid="{27BA6BDA-B2D9-405F-9DD6-DE44F0E7623F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="592" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="688" uniqueCount="106">
   <si>
     <t>F</t>
   </si>
@@ -195,9 +195,6 @@
     <t>Fail action</t>
   </si>
   <si>
-    <t>Sand</t>
-  </si>
-  <si>
     <t>composite</t>
   </si>
   <si>
@@ -316,6 +313,45 @@
   </si>
   <si>
     <t>Analysis, composition</t>
+  </si>
+  <si>
+    <t>Viscosity</t>
+  </si>
+  <si>
+    <t>cP</t>
+  </si>
+  <si>
+    <t>Specific Gravity</t>
+  </si>
+  <si>
+    <t>Heat capacity</t>
+  </si>
+  <si>
+    <t>Semantic ID</t>
+  </si>
+  <si>
+    <t>Head, downstream</t>
+  </si>
+  <si>
+    <t>m</t>
+  </si>
+  <si>
+    <t>Power</t>
+  </si>
+  <si>
+    <t>W, kW, MW</t>
+  </si>
+  <si>
+    <t>Sand, distribution</t>
+  </si>
+  <si>
+    <t>Sand, mass flow</t>
+  </si>
+  <si>
+    <t>kg/h</t>
+  </si>
+  <si>
+    <t>kJ/kg•°C, kJ/kg•°K</t>
   </si>
 </sst>
 </file>
@@ -365,7 +401,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -384,6 +420,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -397,7 +439,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -427,6 +469,10 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -741,11 +787,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA3A2E86-740E-463B-8634-40171DCA62CE}">
-  <dimension ref="A1:N90"/>
+  <dimension ref="A1:O105"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2:N2"/>
+      <pane ySplit="1" topLeftCell="A56" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="Q74" sqref="Q74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -763,9 +809,10 @@
     <col min="12" max="12" width="3.42578125" style="5" customWidth="1"/>
     <col min="13" max="13" width="1.85546875" style="5" customWidth="1"/>
     <col min="14" max="14" width="19.140625" customWidth="1"/>
+    <col min="15" max="15" width="18.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -802,10 +849,13 @@
       <c r="N1" s="4" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="2" spans="1:14" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O1" s="13" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B2" s="12"/>
       <c r="C2" s="12"/>
@@ -820,8 +870,9 @@
       <c r="L2" s="12"/>
       <c r="M2" s="12"/>
       <c r="N2" s="12"/>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O2" s="14"/>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>32</v>
       </c>
@@ -847,7 +898,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>32</v>
       </c>
@@ -858,7 +909,7 @@
         <v>10</v>
       </c>
       <c r="F4" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="G4" t="s">
         <v>34</v>
@@ -873,7 +924,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>32</v>
       </c>
@@ -884,7 +935,7 @@
         <v>10</v>
       </c>
       <c r="F5" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="G5" t="s">
         <v>34</v>
@@ -899,18 +950,18 @@
         <v>47</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>32</v>
       </c>
       <c r="C6" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D6" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="F6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G6" t="s">
         <v>34</v>
@@ -918,14 +969,14 @@
       <c r="H6" t="s">
         <v>45</v>
       </c>
-      <c r="I6" s="5" t="s">
+      <c r="J6" s="5" t="s">
         <v>16</v>
       </c>
       <c r="N6" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>32</v>
       </c>
@@ -936,7 +987,7 @@
         <v>15</v>
       </c>
       <c r="F7" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="G7" t="s">
         <v>34</v>
@@ -951,7 +1002,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>32</v>
       </c>
@@ -962,7 +1013,7 @@
         <v>15</v>
       </c>
       <c r="F8" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="G8" t="s">
         <v>34</v>
@@ -977,18 +1028,18 @@
         <v>47</v>
       </c>
     </row>
-    <row r="9" spans="1:14" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="6" t="s">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>32</v>
       </c>
-      <c r="C9" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="D9" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="F9" s="6" t="s">
-        <v>13</v>
+      <c r="C9" t="s">
+        <v>9</v>
+      </c>
+      <c r="D9" t="s">
+        <v>15</v>
+      </c>
+      <c r="F9" t="s">
+        <v>8</v>
       </c>
       <c r="G9" t="s">
         <v>34</v>
@@ -996,44 +1047,44 @@
       <c r="H9" t="s">
         <v>45</v>
       </c>
-      <c r="I9" s="7"/>
-      <c r="J9" s="7"/>
-      <c r="K9" s="7"/>
-      <c r="L9" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="M9" s="7"/>
+      <c r="I9" s="5" t="s">
+        <v>16</v>
+      </c>
       <c r="N9" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>33</v>
-      </c>
-      <c r="C11" t="s">
-        <v>18</v>
-      </c>
-      <c r="D11" t="s">
-        <v>12</v>
-      </c>
-      <c r="F11" t="s">
-        <v>7</v>
-      </c>
-      <c r="G11" t="s">
-        <v>19</v>
-      </c>
-      <c r="H11" t="s">
-        <v>35</v>
-      </c>
-      <c r="I11" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="N11" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="F10" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G10" t="s">
+        <v>34</v>
+      </c>
+      <c r="H10" t="s">
+        <v>45</v>
+      </c>
+      <c r="I10" s="7"/>
+      <c r="J10" s="7"/>
+      <c r="K10" s="7"/>
+      <c r="L10" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="M10" s="7"/>
+      <c r="N10" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>33</v>
       </c>
@@ -1041,10 +1092,10 @@
         <v>18</v>
       </c>
       <c r="D12" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="F12" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="G12" t="s">
         <v>19</v>
@@ -1052,14 +1103,14 @@
       <c r="H12" t="s">
         <v>35</v>
       </c>
-      <c r="J12" s="5" t="s">
+      <c r="I12" s="5" t="s">
         <v>16</v>
       </c>
       <c r="N12" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>33</v>
       </c>
@@ -1070,7 +1121,7 @@
         <v>10</v>
       </c>
       <c r="F13" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="G13" t="s">
         <v>19</v>
@@ -1085,18 +1136,18 @@
         <v>47</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>33</v>
       </c>
       <c r="C14" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="D14" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="F14" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G14" t="s">
         <v>19</v>
@@ -1104,14 +1155,14 @@
       <c r="H14" t="s">
         <v>35</v>
       </c>
-      <c r="I14" s="5" t="s">
+      <c r="J14" s="5" t="s">
         <v>16</v>
       </c>
       <c r="N14" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>33</v>
       </c>
@@ -1122,7 +1173,7 @@
         <v>15</v>
       </c>
       <c r="F15" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="G15" t="s">
         <v>19</v>
@@ -1137,7 +1188,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>33</v>
       </c>
@@ -1148,7 +1199,7 @@
         <v>15</v>
       </c>
       <c r="F16" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="G16" t="s">
         <v>19</v>
@@ -1163,82 +1214,82 @@
         <v>47</v>
       </c>
     </row>
-    <row r="17" spans="1:14" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="6" t="s">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
         <v>33</v>
       </c>
-      <c r="C17" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="D17" s="6" t="s">
+      <c r="C17" t="s">
+        <v>9</v>
+      </c>
+      <c r="D17" t="s">
+        <v>15</v>
+      </c>
+      <c r="F17" t="s">
+        <v>8</v>
+      </c>
+      <c r="G17" t="s">
+        <v>19</v>
+      </c>
+      <c r="H17" t="s">
+        <v>35</v>
+      </c>
+      <c r="I17" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="N17" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D18" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="F17" s="6" t="s">
+      <c r="F18" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="G17" s="6" t="s">
+      <c r="G18" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="H17" s="6" t="s">
+      <c r="H18" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="I17" s="7"/>
-      <c r="J17" s="7"/>
-      <c r="K17" s="7"/>
-      <c r="L17" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="M17" s="7"/>
-      <c r="N17" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="18" spans="1:14" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="I18" s="7"/>
       <c r="J18" s="7"/>
       <c r="K18" s="7"/>
-      <c r="L18" s="7"/>
+      <c r="L18" s="7" t="s">
+        <v>16</v>
+      </c>
       <c r="M18" s="7"/>
-      <c r="N18"/>
-    </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>60</v>
-      </c>
-      <c r="C19" t="s">
-        <v>18</v>
-      </c>
-      <c r="D19" t="s">
-        <v>12</v>
-      </c>
-      <c r="F19" t="s">
-        <v>8</v>
-      </c>
-      <c r="G19" t="s">
-        <v>19</v>
-      </c>
-      <c r="H19" t="s">
-        <v>35</v>
-      </c>
-      <c r="I19" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="N19" t="s">
-        <v>47</v>
-      </c>
+      <c r="N18" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I19" s="7"/>
+      <c r="J19" s="7"/>
+      <c r="K19" s="7"/>
+      <c r="L19" s="7"/>
+      <c r="M19" s="7"/>
+      <c r="N19"/>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C20" t="s">
         <v>18</v>
       </c>
       <c r="D20" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="F20" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="G20" t="s">
         <v>19</v>
@@ -1246,7 +1297,7 @@
       <c r="H20" t="s">
         <v>35</v>
       </c>
-      <c r="J20" s="5" t="s">
+      <c r="I20" s="5" t="s">
         <v>16</v>
       </c>
       <c r="N20" t="s">
@@ -1255,7 +1306,7 @@
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C21" t="s">
         <v>18</v>
@@ -1264,7 +1315,7 @@
         <v>10</v>
       </c>
       <c r="F21" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="G21" t="s">
         <v>19</v>
@@ -1281,16 +1332,16 @@
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C22" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="D22" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="F22" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G22" t="s">
         <v>19</v>
@@ -1298,7 +1349,7 @@
       <c r="H22" t="s">
         <v>35</v>
       </c>
-      <c r="I22" s="5" t="s">
+      <c r="J22" s="5" t="s">
         <v>16</v>
       </c>
       <c r="N22" t="s">
@@ -1307,7 +1358,7 @@
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C23" t="s">
         <v>9</v>
@@ -1316,7 +1367,7 @@
         <v>15</v>
       </c>
       <c r="F23" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="G23" t="s">
         <v>19</v>
@@ -1333,7 +1384,7 @@
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C24" t="s">
         <v>9</v>
@@ -1342,7 +1393,7 @@
         <v>15</v>
       </c>
       <c r="F24" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="G24" t="s">
         <v>19</v>
@@ -1357,60 +1408,60 @@
         <v>47</v>
       </c>
     </row>
-    <row r="25" spans="1:14" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="9" t="s">
-        <v>60</v>
-      </c>
-      <c r="C25" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="D25" s="6" t="s">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>59</v>
+      </c>
+      <c r="C25" t="s">
+        <v>9</v>
+      </c>
+      <c r="D25" t="s">
+        <v>15</v>
+      </c>
+      <c r="F25" t="s">
+        <v>8</v>
+      </c>
+      <c r="G25" t="s">
+        <v>19</v>
+      </c>
+      <c r="H25" t="s">
+        <v>35</v>
+      </c>
+      <c r="I25" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="N25" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="C26" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D26" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="F25" s="6" t="s">
+      <c r="F26" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="G25" s="6" t="s">
+      <c r="G26" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="H25" s="6" t="s">
+      <c r="H26" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="I25" s="7"/>
-      <c r="J25" s="7"/>
-      <c r="K25" s="7"/>
-      <c r="L25" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="M25" s="7"/>
-      <c r="N25" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>22</v>
-      </c>
-      <c r="C27" t="s">
-        <v>18</v>
-      </c>
-      <c r="D27" t="s">
-        <v>24</v>
-      </c>
-      <c r="F27" t="s">
-        <v>7</v>
-      </c>
-      <c r="G27" t="s">
-        <v>29</v>
-      </c>
-      <c r="H27" t="s">
-        <v>23</v>
-      </c>
-      <c r="I27" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="N27" t="s">
-        <v>48</v>
+      <c r="I26" s="7"/>
+      <c r="J26" s="7"/>
+      <c r="K26" s="7"/>
+      <c r="L26" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="M26" s="7"/>
+      <c r="N26" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.25">
@@ -1421,7 +1472,7 @@
         <v>18</v>
       </c>
       <c r="D28" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F28" t="s">
         <v>7</v>
@@ -1447,10 +1498,10 @@
         <v>18</v>
       </c>
       <c r="D29" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="F29" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="G29" t="s">
         <v>29</v>
@@ -1458,7 +1509,7 @@
       <c r="H29" t="s">
         <v>23</v>
       </c>
-      <c r="J29" s="5" t="s">
+      <c r="I29" s="5" t="s">
         <v>16</v>
       </c>
       <c r="N29" t="s">
@@ -1476,7 +1527,7 @@
         <v>27</v>
       </c>
       <c r="F30" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="G30" t="s">
         <v>29</v>
@@ -1499,10 +1550,10 @@
         <v>18</v>
       </c>
       <c r="D31" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F31" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="G31" t="s">
         <v>29</v>
@@ -1528,7 +1579,7 @@
         <v>28</v>
       </c>
       <c r="F32" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="G32" t="s">
         <v>29</v>
@@ -1548,13 +1599,13 @@
         <v>22</v>
       </c>
       <c r="C33" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="D33" t="s">
-        <v>15</v>
+        <v>28</v>
       </c>
       <c r="F33" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G33" t="s">
         <v>29</v>
@@ -1562,7 +1613,7 @@
       <c r="H33" t="s">
         <v>23</v>
       </c>
-      <c r="I33" s="5" t="s">
+      <c r="J33" s="5" t="s">
         <v>16</v>
       </c>
       <c r="N33" t="s">
@@ -1580,7 +1631,7 @@
         <v>15</v>
       </c>
       <c r="F34" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="G34" t="s">
         <v>29</v>
@@ -1606,7 +1657,7 @@
         <v>15</v>
       </c>
       <c r="F35" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="G35" t="s">
         <v>29</v>
@@ -1621,60 +1672,60 @@
         <v>48</v>
       </c>
     </row>
-    <row r="36" spans="1:14" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="6" t="s">
+    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
         <v>22</v>
       </c>
-      <c r="C36" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="D36" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="F36" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="G36" s="6" t="s">
+      <c r="C36" t="s">
+        <v>9</v>
+      </c>
+      <c r="D36" t="s">
+        <v>15</v>
+      </c>
+      <c r="F36" t="s">
+        <v>8</v>
+      </c>
+      <c r="G36" t="s">
         <v>29</v>
       </c>
-      <c r="H36" s="6" t="s">
+      <c r="H36" t="s">
         <v>23</v>
       </c>
-      <c r="I36" s="7"/>
-      <c r="J36" s="7"/>
-      <c r="K36" s="7"/>
-      <c r="L36" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="M36" s="7"/>
+      <c r="I36" s="5" t="s">
+        <v>16</v>
+      </c>
       <c r="N36" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>30</v>
-      </c>
-      <c r="C38" t="s">
-        <v>18</v>
-      </c>
-      <c r="D38" t="s">
-        <v>24</v>
-      </c>
-      <c r="F38" t="s">
-        <v>7</v>
-      </c>
-      <c r="G38" t="s">
+    <row r="37" spans="1:14" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C37" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D37" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="F37" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G37" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="H38" t="s">
-        <v>31</v>
-      </c>
-      <c r="I38" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="N38" t="s">
-        <v>49</v>
+      <c r="H37" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="I37" s="7"/>
+      <c r="J37" s="7"/>
+      <c r="K37" s="7"/>
+      <c r="L37" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="M37" s="7"/>
+      <c r="N37" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="39" spans="1:14" x14ac:dyDescent="0.25">
@@ -1685,7 +1736,7 @@
         <v>18</v>
       </c>
       <c r="D39" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F39" t="s">
         <v>7</v>
@@ -1711,10 +1762,10 @@
         <v>18</v>
       </c>
       <c r="D40" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="F40" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="G40" t="s">
         <v>29</v>
@@ -1722,7 +1773,7 @@
       <c r="H40" t="s">
         <v>31</v>
       </c>
-      <c r="J40" s="5" t="s">
+      <c r="I40" s="5" t="s">
         <v>16</v>
       </c>
       <c r="N40" t="s">
@@ -1737,7 +1788,7 @@
         <v>18</v>
       </c>
       <c r="D41" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F41" t="s">
         <v>11</v>
@@ -1760,13 +1811,13 @@
         <v>30</v>
       </c>
       <c r="C42" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="D42" t="s">
-        <v>15</v>
+        <v>28</v>
       </c>
       <c r="F42" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="G42" t="s">
         <v>29</v>
@@ -1774,7 +1825,7 @@
       <c r="H42" t="s">
         <v>31</v>
       </c>
-      <c r="I42" s="5" t="s">
+      <c r="J42" s="5" t="s">
         <v>16</v>
       </c>
       <c r="N42" t="s">
@@ -1792,7 +1843,7 @@
         <v>15</v>
       </c>
       <c r="F43" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="G43" t="s">
         <v>29</v>
@@ -1818,7 +1869,7 @@
         <v>15</v>
       </c>
       <c r="F44" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="G44" t="s">
         <v>29</v>
@@ -1833,60 +1884,60 @@
         <v>49</v>
       </c>
     </row>
-    <row r="45" spans="1:14" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="6" t="s">
+    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
         <v>30</v>
       </c>
-      <c r="C45" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="D45" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="F45" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="G45" s="6" t="s">
+      <c r="C45" t="s">
+        <v>9</v>
+      </c>
+      <c r="D45" t="s">
+        <v>15</v>
+      </c>
+      <c r="F45" t="s">
+        <v>8</v>
+      </c>
+      <c r="G45" t="s">
         <v>29</v>
       </c>
-      <c r="H45" s="6" t="s">
+      <c r="H45" t="s">
         <v>31</v>
       </c>
-      <c r="I45" s="7"/>
-      <c r="J45" s="7"/>
-      <c r="K45" s="7"/>
-      <c r="L45" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="M45" s="7"/>
+      <c r="I45" s="5" t="s">
+        <v>16</v>
+      </c>
       <c r="N45" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
-        <v>36</v>
-      </c>
-      <c r="C47" t="s">
-        <v>9</v>
-      </c>
-      <c r="D47" t="s">
-        <v>15</v>
-      </c>
-      <c r="F47" t="s">
-        <v>7</v>
-      </c>
-      <c r="G47" t="s">
+    <row r="46" spans="1:14" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="C46" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D46" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="F46" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G46" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="H47" t="s">
-        <v>37</v>
-      </c>
-      <c r="I47" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="N47" t="s">
-        <v>47</v>
+      <c r="H46" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="I46" s="7"/>
+      <c r="J46" s="7"/>
+      <c r="K46" s="7"/>
+      <c r="L46" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="M46" s="7"/>
+      <c r="N46" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="48" spans="1:14" x14ac:dyDescent="0.25">
@@ -1900,7 +1951,7 @@
         <v>15</v>
       </c>
       <c r="F48" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="G48" t="s">
         <v>29</v>
@@ -1926,7 +1977,7 @@
         <v>15</v>
       </c>
       <c r="F49" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="G49" t="s">
         <v>29</v>
@@ -1942,217 +1993,228 @@
       </c>
     </row>
     <row r="50" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A50" s="6" t="s">
+      <c r="A50" t="s">
         <v>36</v>
       </c>
-      <c r="C50" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="D50" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="E50" s="6"/>
-      <c r="F50" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="G50" s="6" t="s">
+      <c r="C50" t="s">
+        <v>9</v>
+      </c>
+      <c r="D50" t="s">
+        <v>15</v>
+      </c>
+      <c r="F50" t="s">
+        <v>8</v>
+      </c>
+      <c r="G50" t="s">
         <v>29</v>
       </c>
       <c r="H50" t="s">
         <v>37</v>
       </c>
-      <c r="L50" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="M50" s="7"/>
+      <c r="I50" s="5" t="s">
+        <v>16</v>
+      </c>
       <c r="N50" t="s">
         <v>47</v>
       </c>
     </row>
+    <row r="51" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A51" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="C51" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D51" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="E51" s="6"/>
+      <c r="F51" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G51" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="H51" t="s">
+        <v>37</v>
+      </c>
+      <c r="L51" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="M51" s="7"/>
+      <c r="N51" t="s">
+        <v>47</v>
+      </c>
+    </row>
     <row r="52" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
-        <v>38</v>
-      </c>
-      <c r="C52" t="s">
-        <v>9</v>
-      </c>
-      <c r="D52" t="s">
-        <v>15</v>
-      </c>
-      <c r="F52" t="s">
-        <v>11</v>
-      </c>
-      <c r="H52" t="s">
-        <v>42</v>
-      </c>
-      <c r="I52" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="N52" t="s">
-        <v>49</v>
-      </c>
+      <c r="A52" s="6"/>
+      <c r="C52" s="6"/>
+      <c r="D52" s="6"/>
+      <c r="E52" s="6"/>
+      <c r="F52" s="6"/>
+      <c r="G52" s="6"/>
+      <c r="L52" s="7"/>
+      <c r="M52" s="7"/>
     </row>
     <row r="53" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
-        <v>39</v>
+      <c r="A53" s="10" t="s">
+        <v>100</v>
       </c>
       <c r="C53" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D53" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="F53" t="s">
-        <v>11</v>
-      </c>
+        <v>7</v>
+      </c>
+      <c r="G53" s="6"/>
       <c r="H53" t="s">
-        <v>42</v>
-      </c>
-      <c r="I53" s="5" t="s">
-        <v>16</v>
-      </c>
+        <v>101</v>
+      </c>
+      <c r="L53" s="7"/>
+      <c r="M53" s="7"/>
       <c r="N53" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="54" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
-        <v>40</v>
+      <c r="A54" s="10" t="s">
+        <v>100</v>
       </c>
       <c r="C54" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D54" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="F54" t="s">
         <v>11</v>
       </c>
+      <c r="G54" s="6"/>
       <c r="H54" t="s">
-        <v>42</v>
-      </c>
-      <c r="I54" s="5" t="s">
-        <v>16</v>
-      </c>
+        <v>101</v>
+      </c>
+      <c r="L54" s="7"/>
+      <c r="M54" s="7"/>
       <c r="N54" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="55" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
-        <v>41</v>
+      <c r="A55" s="10" t="s">
+        <v>100</v>
       </c>
       <c r="C55" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D55" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="F55" t="s">
+        <v>8</v>
+      </c>
+      <c r="G55" s="6"/>
+      <c r="H55" t="s">
+        <v>101</v>
+      </c>
+      <c r="L55" s="7"/>
+      <c r="M55" s="7"/>
+      <c r="N55" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="56" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A56" s="10" t="s">
+        <v>100</v>
+      </c>
+      <c r="C56" t="s">
+        <v>9</v>
+      </c>
+      <c r="D56" t="s">
+        <v>15</v>
+      </c>
+      <c r="F56" t="s">
+        <v>7</v>
+      </c>
+      <c r="G56" s="6"/>
+      <c r="H56" t="s">
+        <v>101</v>
+      </c>
+      <c r="L56" s="7"/>
+      <c r="M56" s="7"/>
+      <c r="N56" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="57" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A57" s="10" t="s">
+        <v>100</v>
+      </c>
+      <c r="C57" t="s">
+        <v>9</v>
+      </c>
+      <c r="D57" t="s">
+        <v>15</v>
+      </c>
+      <c r="F57" t="s">
         <v>11</v>
       </c>
-      <c r="H55" t="s">
-        <v>42</v>
-      </c>
-      <c r="I55" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="N55" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="56" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
-        <v>59</v>
-      </c>
-      <c r="C56" t="s">
-        <v>9</v>
-      </c>
-      <c r="D56" t="s">
-        <v>15</v>
-      </c>
-      <c r="F56" t="s">
-        <v>11</v>
-      </c>
-      <c r="H56" t="s">
-        <v>58</v>
-      </c>
-      <c r="I56" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="N56" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="57" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A57" t="s">
-        <v>74</v>
-      </c>
-      <c r="C57" t="s">
-        <v>18</v>
-      </c>
-      <c r="D57" t="s">
-        <v>12</v>
-      </c>
-      <c r="F57" t="s">
-        <v>8</v>
-      </c>
+      <c r="G57" s="6"/>
       <c r="H57" t="s">
-        <v>73</v>
-      </c>
-      <c r="I57" s="5" t="s">
-        <v>16</v>
-      </c>
+        <v>101</v>
+      </c>
+      <c r="L57" s="7"/>
+      <c r="M57" s="7"/>
       <c r="N57" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="58" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A58" t="s">
-        <v>75</v>
+      <c r="A58" s="10" t="s">
+        <v>100</v>
       </c>
       <c r="C58" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="D58" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="F58" t="s">
         <v>8</v>
       </c>
+      <c r="G58" s="6"/>
       <c r="H58" t="s">
-        <v>76</v>
-      </c>
-      <c r="I58" s="5" t="s">
-        <v>16</v>
-      </c>
+        <v>101</v>
+      </c>
+      <c r="L58" s="7"/>
+      <c r="M58" s="7"/>
       <c r="N58" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="60" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A60" t="s">
-        <v>43</v>
-      </c>
-      <c r="C60" t="s">
-        <v>18</v>
-      </c>
-      <c r="D60" t="s">
-        <v>12</v>
-      </c>
-      <c r="F60" t="s">
-        <v>7</v>
-      </c>
-      <c r="G60" t="s">
-        <v>29</v>
-      </c>
-      <c r="H60" t="s">
-        <v>44</v>
-      </c>
-      <c r="I60" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="N60" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="59" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A59" s="10" t="s">
+        <v>100</v>
+      </c>
+      <c r="C59" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D59" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="E59" s="6"/>
+      <c r="F59" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G59" s="6"/>
+      <c r="H59" t="s">
+        <v>101</v>
+      </c>
+      <c r="L59" s="7"/>
+      <c r="M59" s="7"/>
+      <c r="N59" t="s">
         <v>47</v>
       </c>
     </row>
@@ -2167,7 +2229,7 @@
         <v>12</v>
       </c>
       <c r="F61" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G61" t="s">
         <v>29</v>
@@ -2190,10 +2252,10 @@
         <v>18</v>
       </c>
       <c r="D62" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="F62" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G62" t="s">
         <v>29</v>
@@ -2201,7 +2263,7 @@
       <c r="H62" t="s">
         <v>44</v>
       </c>
-      <c r="J62" s="5" t="s">
+      <c r="I62" s="5" t="s">
         <v>16</v>
       </c>
       <c r="N62" t="s">
@@ -2219,7 +2281,7 @@
         <v>10</v>
       </c>
       <c r="F63" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G63" t="s">
         <v>29</v>
@@ -2239,13 +2301,13 @@
         <v>43</v>
       </c>
       <c r="C64" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="D64" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="F64" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G64" t="s">
         <v>29</v>
@@ -2253,7 +2315,7 @@
       <c r="H64" t="s">
         <v>44</v>
       </c>
-      <c r="I64" s="5" t="s">
+      <c r="J64" s="5" t="s">
         <v>16</v>
       </c>
       <c r="N64" t="s">
@@ -2271,7 +2333,7 @@
         <v>15</v>
       </c>
       <c r="F65" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="G65" t="s">
         <v>29</v>
@@ -2297,7 +2359,7 @@
         <v>15</v>
       </c>
       <c r="F66" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="G66" t="s">
         <v>29</v>
@@ -2312,202 +2374,269 @@
         <v>47</v>
       </c>
     </row>
+    <row r="67" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>43</v>
+      </c>
+      <c r="C67" t="s">
+        <v>9</v>
+      </c>
+      <c r="D67" t="s">
+        <v>15</v>
+      </c>
+      <c r="F67" t="s">
+        <v>8</v>
+      </c>
+      <c r="G67" t="s">
+        <v>29</v>
+      </c>
+      <c r="H67" t="s">
+        <v>44</v>
+      </c>
+      <c r="I67" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="N67" t="s">
+        <v>47</v>
+      </c>
+    </row>
     <row r="68" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A68" s="9" t="s">
-        <v>53</v>
-      </c>
-      <c r="C68" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="D68" s="6" t="s">
-        <v>14</v>
-      </c>
+      <c r="A68" s="6"/>
+      <c r="C68" s="6"/>
+      <c r="D68" s="6"/>
       <c r="E68" s="6"/>
-      <c r="F68" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="H68" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="L68" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="N68" s="9" t="s">
-        <v>55</v>
-      </c>
+      <c r="F68" s="6"/>
+      <c r="G68" s="6"/>
+      <c r="L68" s="7"/>
+      <c r="M68" s="7"/>
     </row>
     <row r="69" spans="1:14" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A69" s="10" t="s">
-        <v>93</v>
+        <v>103</v>
       </c>
       <c r="C69" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="D69" t="s">
-        <v>15</v>
-      </c>
-      <c r="F69" t="s">
-        <v>11</v>
+        <v>18</v>
+      </c>
+      <c r="D69" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F69" s="10" t="s">
+        <v>8</v>
       </c>
       <c r="H69" s="10" t="s">
-        <v>54</v>
-      </c>
-      <c r="I69" s="11"/>
+        <v>104</v>
+      </c>
+      <c r="I69" s="11" t="s">
+        <v>16</v>
+      </c>
       <c r="J69" s="11"/>
       <c r="K69" s="11"/>
-      <c r="L69" s="11" t="s">
-        <v>16</v>
-      </c>
+      <c r="L69" s="11"/>
       <c r="M69" s="11"/>
       <c r="N69" s="10" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="70" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A70" s="9" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="70" spans="1:14" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A70" s="10" t="s">
+        <v>103</v>
+      </c>
+      <c r="C70" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="D70" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F70" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="H70" s="10" t="s">
+        <v>104</v>
+      </c>
+      <c r="I70" s="11"/>
+      <c r="J70" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="K70" s="11"/>
+      <c r="L70" s="11"/>
+      <c r="M70" s="11"/>
+      <c r="N70" s="10" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="71" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A71" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="C71" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D71" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="E71" s="6"/>
+      <c r="F71" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="H71" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="L71" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="N71" s="9" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="72" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A72" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="C72" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D72" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="E72" s="6"/>
+      <c r="F72" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="H72" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="L72" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="N72" s="9" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="73" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A73" s="9"/>
+      <c r="C73" s="6"/>
+      <c r="D73" s="6"/>
+      <c r="E73" s="6"/>
+      <c r="F73" s="6"/>
+      <c r="H73" s="6"/>
+      <c r="L73" s="8"/>
+      <c r="N73" s="9"/>
+    </row>
+    <row r="74" spans="1:14" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A74" s="10" t="s">
         <v>93</v>
       </c>
-      <c r="C70" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="D70" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="E70" s="6"/>
-      <c r="F70" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="H70" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="L70" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="N70" s="9" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="73" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A73" t="s">
-        <v>50</v>
-      </c>
-      <c r="C73" t="s">
-        <v>18</v>
-      </c>
-      <c r="D73" t="s">
-        <v>12</v>
-      </c>
-      <c r="F73" t="s">
-        <v>11</v>
-      </c>
-      <c r="H73" t="s">
-        <v>79</v>
-      </c>
-      <c r="I73" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="J73" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="N73" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="74" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A74" t="s">
-        <v>66</v>
-      </c>
       <c r="C74" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="D74" t="s">
-        <v>12</v>
-      </c>
+        <v>15</v>
+      </c>
+      <c r="E74"/>
       <c r="F74" t="s">
         <v>11</v>
       </c>
-      <c r="H74" t="s">
-        <v>42</v>
-      </c>
+      <c r="H74" s="10" t="s">
+        <v>94</v>
+      </c>
+      <c r="I74" s="11"/>
+      <c r="J74" s="11"/>
+      <c r="K74" s="11"/>
+      <c r="L74" s="11"/>
+      <c r="M74" s="11"/>
       <c r="N74" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="75" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A75" t="s">
-        <v>51</v>
+        <v>47</v>
+      </c>
+    </row>
+    <row r="75" spans="1:14" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A75" s="10" t="s">
+        <v>95</v>
       </c>
       <c r="C75" t="s">
         <v>9</v>
       </c>
       <c r="D75" t="s">
-        <v>12</v>
-      </c>
+        <v>15</v>
+      </c>
+      <c r="E75"/>
       <c r="F75" t="s">
         <v>11</v>
       </c>
-      <c r="H75" t="s">
-        <v>80</v>
-      </c>
+      <c r="H75" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="I75" s="11"/>
+      <c r="J75" s="11"/>
+      <c r="K75" s="11"/>
+      <c r="L75" s="11"/>
+      <c r="M75" s="11"/>
       <c r="N75" t="s">
-        <v>90</v>
+        <v>49</v>
       </c>
     </row>
     <row r="76" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A76" t="s">
-        <v>52</v>
+      <c r="A76" s="10" t="s">
+        <v>96</v>
       </c>
       <c r="C76" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="D76" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="F76" t="s">
         <v>11</v>
       </c>
       <c r="H76" t="s">
-        <v>81</v>
-      </c>
+        <v>105</v>
+      </c>
+      <c r="L76" s="7"/>
+      <c r="M76" s="7"/>
       <c r="N76" t="s">
-        <v>78</v>
+        <v>47</v>
       </c>
     </row>
     <row r="77" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A77" t="s">
-        <v>82</v>
+      <c r="A77" s="10" t="s">
+        <v>98</v>
       </c>
       <c r="C77" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="D77" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="F77" t="s">
-        <v>7</v>
-      </c>
+        <v>11</v>
+      </c>
+      <c r="G77" s="6"/>
       <c r="H77" t="s">
-        <v>84</v>
-      </c>
+        <v>99</v>
+      </c>
+      <c r="L77" s="7"/>
+      <c r="M77" s="7"/>
       <c r="N77" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="78" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>83</v>
+        <v>38</v>
       </c>
       <c r="C78" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="D78" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="F78" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="H78" t="s">
-        <v>84</v>
+        <v>42</v>
+      </c>
+      <c r="I78" s="5" t="s">
+        <v>16</v>
       </c>
       <c r="N78" t="s">
         <v>49</v>
@@ -2515,79 +2644,91 @@
     </row>
     <row r="79" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>89</v>
+        <v>39</v>
       </c>
       <c r="C79" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="D79" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="F79" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="H79" t="s">
-        <v>77</v>
+        <v>42</v>
+      </c>
+      <c r="I79" s="5" t="s">
+        <v>16</v>
       </c>
       <c r="N79" t="s">
-        <v>91</v>
+        <v>49</v>
       </c>
     </row>
     <row r="80" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>56</v>
+        <v>40</v>
       </c>
       <c r="C80" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="D80" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="F80" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="H80" t="s">
         <v>42</v>
       </c>
+      <c r="I80" s="5" t="s">
+        <v>16</v>
+      </c>
       <c r="N80" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="81" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>57</v>
+        <v>41</v>
       </c>
       <c r="C81" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="D81" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="F81" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="H81" t="s">
         <v>42</v>
       </c>
+      <c r="I81" s="5" t="s">
+        <v>16</v>
+      </c>
       <c r="N81" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="82" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C82" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="D82" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="F82" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="H82" t="s">
-        <v>62</v>
+        <v>57</v>
+      </c>
+      <c r="I82" s="5" t="s">
+        <v>16</v>
       </c>
       <c r="N82" t="s">
         <v>47</v>
@@ -2595,7 +2736,7 @@
     </row>
     <row r="83" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>63</v>
+        <v>73</v>
       </c>
       <c r="C83" t="s">
         <v>18</v>
@@ -2607,7 +2748,10 @@
         <v>8</v>
       </c>
       <c r="H83" t="s">
-        <v>42</v>
+        <v>72</v>
+      </c>
+      <c r="I83" s="5" t="s">
+        <v>16</v>
       </c>
       <c r="N83" t="s">
         <v>49</v>
@@ -2615,7 +2759,7 @@
     </row>
     <row r="84" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>64</v>
+        <v>74</v>
       </c>
       <c r="C84" t="s">
         <v>18</v>
@@ -2627,75 +2771,69 @@
         <v>8</v>
       </c>
       <c r="H84" t="s">
-        <v>65</v>
+        <v>75</v>
+      </c>
+      <c r="I84" s="5" t="s">
+        <v>16</v>
       </c>
       <c r="N84" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="85" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A85" t="s">
-        <v>69</v>
-      </c>
-      <c r="C85" t="s">
-        <v>18</v>
+        <v>49</v>
+      </c>
+    </row>
+    <row r="85" spans="1:14" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A85" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="C85" s="10" t="s">
+        <v>9</v>
       </c>
       <c r="D85" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="F85" t="s">
-        <v>8</v>
-      </c>
-      <c r="H85" t="s">
-        <v>70</v>
-      </c>
-      <c r="N85" t="s">
-        <v>47</v>
+        <v>11</v>
+      </c>
+      <c r="H85" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="I85" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="J85" s="11"/>
+      <c r="K85" s="11"/>
+      <c r="L85" s="11"/>
+      <c r="M85" s="11"/>
+      <c r="N85" s="10" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="86" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A86" t="s">
-        <v>67</v>
-      </c>
-      <c r="C86" t="s">
-        <v>18</v>
-      </c>
-      <c r="D86" t="s">
-        <v>12</v>
-      </c>
-      <c r="F86" t="s">
-        <v>8</v>
-      </c>
-      <c r="H86" t="s">
-        <v>68</v>
-      </c>
-      <c r="N86" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="87" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A87" t="s">
-        <v>71</v>
-      </c>
-      <c r="C87" t="s">
-        <v>18</v>
-      </c>
-      <c r="D87" t="s">
-        <v>12</v>
-      </c>
-      <c r="F87" t="s">
-        <v>7</v>
-      </c>
-      <c r="H87" t="s">
-        <v>72</v>
-      </c>
-      <c r="N87" t="s">
-        <v>49</v>
+      <c r="A86" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="C86" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D86" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="E86" s="6"/>
+      <c r="F86" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="H86" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="L86" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="N86" s="9" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="88" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>71</v>
+        <v>50</v>
       </c>
       <c r="C88" t="s">
         <v>18</v>
@@ -2704,38 +2842,44 @@
         <v>12</v>
       </c>
       <c r="F88" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="H88" t="s">
-        <v>72</v>
+        <v>78</v>
+      </c>
+      <c r="I88" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="J88" s="5" t="s">
+        <v>16</v>
       </c>
       <c r="N88" t="s">
-        <v>49</v>
+        <v>77</v>
       </c>
     </row>
     <row r="89" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>85</v>
+        <v>65</v>
       </c>
       <c r="C89" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="D89" t="s">
         <v>12</v>
       </c>
       <c r="F89" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="H89" t="s">
-        <v>87</v>
+        <v>42</v>
       </c>
       <c r="N89" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
     </row>
     <row r="90" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>86</v>
+        <v>51</v>
       </c>
       <c r="C90" t="s">
         <v>9</v>
@@ -2744,12 +2888,312 @@
         <v>12</v>
       </c>
       <c r="F90" t="s">
+        <v>11</v>
+      </c>
+      <c r="H90" t="s">
+        <v>79</v>
+      </c>
+      <c r="N90" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="91" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>52</v>
+      </c>
+      <c r="C91" t="s">
+        <v>18</v>
+      </c>
+      <c r="D91" t="s">
+        <v>12</v>
+      </c>
+      <c r="F91" t="s">
+        <v>11</v>
+      </c>
+      <c r="H91" t="s">
+        <v>80</v>
+      </c>
+      <c r="N91" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="92" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>81</v>
+      </c>
+      <c r="C92" t="s">
+        <v>18</v>
+      </c>
+      <c r="D92" t="s">
+        <v>12</v>
+      </c>
+      <c r="F92" t="s">
         <v>7</v>
       </c>
-      <c r="H90" t="s">
+      <c r="H92" t="s">
+        <v>83</v>
+      </c>
+      <c r="N92" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="93" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>82</v>
+      </c>
+      <c r="C93" t="s">
+        <v>18</v>
+      </c>
+      <c r="D93" t="s">
+        <v>12</v>
+      </c>
+      <c r="F93" t="s">
+        <v>7</v>
+      </c>
+      <c r="H93" t="s">
+        <v>83</v>
+      </c>
+      <c r="N93" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="94" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
         <v>88</v>
       </c>
-      <c r="N90" t="s">
+      <c r="C94" t="s">
+        <v>18</v>
+      </c>
+      <c r="D94" t="s">
+        <v>12</v>
+      </c>
+      <c r="F94" t="s">
+        <v>8</v>
+      </c>
+      <c r="H94" t="s">
+        <v>76</v>
+      </c>
+      <c r="N94" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="95" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>55</v>
+      </c>
+      <c r="C95" t="s">
+        <v>18</v>
+      </c>
+      <c r="D95" t="s">
+        <v>12</v>
+      </c>
+      <c r="F95" t="s">
+        <v>7</v>
+      </c>
+      <c r="H95" t="s">
+        <v>42</v>
+      </c>
+      <c r="N95" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="96" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
+        <v>56</v>
+      </c>
+      <c r="C96" t="s">
+        <v>18</v>
+      </c>
+      <c r="D96" t="s">
+        <v>12</v>
+      </c>
+      <c r="F96" t="s">
+        <v>7</v>
+      </c>
+      <c r="H96" t="s">
+        <v>42</v>
+      </c>
+      <c r="N96" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="97" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>60</v>
+      </c>
+      <c r="C97" t="s">
+        <v>18</v>
+      </c>
+      <c r="D97" t="s">
+        <v>12</v>
+      </c>
+      <c r="F97" t="s">
+        <v>7</v>
+      </c>
+      <c r="H97" t="s">
+        <v>61</v>
+      </c>
+      <c r="N97" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="98" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
+        <v>62</v>
+      </c>
+      <c r="C98" t="s">
+        <v>18</v>
+      </c>
+      <c r="D98" t="s">
+        <v>12</v>
+      </c>
+      <c r="F98" t="s">
+        <v>8</v>
+      </c>
+      <c r="H98" t="s">
+        <v>42</v>
+      </c>
+      <c r="N98" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="99" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
+        <v>63</v>
+      </c>
+      <c r="C99" t="s">
+        <v>18</v>
+      </c>
+      <c r="D99" t="s">
+        <v>12</v>
+      </c>
+      <c r="F99" t="s">
+        <v>8</v>
+      </c>
+      <c r="H99" t="s">
+        <v>64</v>
+      </c>
+      <c r="N99" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="100" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
+        <v>68</v>
+      </c>
+      <c r="C100" t="s">
+        <v>18</v>
+      </c>
+      <c r="D100" t="s">
+        <v>12</v>
+      </c>
+      <c r="F100" t="s">
+        <v>8</v>
+      </c>
+      <c r="H100" t="s">
+        <v>69</v>
+      </c>
+      <c r="N100" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="101" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
+        <v>66</v>
+      </c>
+      <c r="C101" t="s">
+        <v>18</v>
+      </c>
+      <c r="D101" t="s">
+        <v>12</v>
+      </c>
+      <c r="F101" t="s">
+        <v>8</v>
+      </c>
+      <c r="H101" t="s">
+        <v>67</v>
+      </c>
+      <c r="N101" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="102" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
+        <v>70</v>
+      </c>
+      <c r="C102" t="s">
+        <v>18</v>
+      </c>
+      <c r="D102" t="s">
+        <v>12</v>
+      </c>
+      <c r="F102" t="s">
+        <v>7</v>
+      </c>
+      <c r="H102" t="s">
+        <v>71</v>
+      </c>
+      <c r="N102" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="103" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A103" t="s">
+        <v>70</v>
+      </c>
+      <c r="C103" t="s">
+        <v>18</v>
+      </c>
+      <c r="D103" t="s">
+        <v>12</v>
+      </c>
+      <c r="F103" t="s">
+        <v>8</v>
+      </c>
+      <c r="H103" t="s">
+        <v>71</v>
+      </c>
+      <c r="N103" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="104" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A104" t="s">
+        <v>84</v>
+      </c>
+      <c r="C104" t="s">
+        <v>9</v>
+      </c>
+      <c r="D104" t="s">
+        <v>12</v>
+      </c>
+      <c r="F104" t="s">
+        <v>7</v>
+      </c>
+      <c r="H104" t="s">
+        <v>86</v>
+      </c>
+      <c r="N104" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="105" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A105" t="s">
+        <v>85</v>
+      </c>
+      <c r="C105" t="s">
+        <v>9</v>
+      </c>
+      <c r="D105" t="s">
+        <v>12</v>
+      </c>
+      <c r="F105" t="s">
+        <v>7</v>
+      </c>
+      <c r="H105" t="s">
+        <v>87</v>
+      </c>
+      <c r="N105" t="s">
         <v>47</v>
       </c>
     </row>
@@ -2759,5 +3203,6 @@
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>